<commit_message>
removed vias on high current trace, and regenerated gerbers + output files.
</commit_message>
<xml_diff>
--- a/MSXIV_SolarSense/MSXIV_SolarSense/Project Outputs for MSXIV_SolarSense/BOM&STEP/MSXIV_SolarSense_1.0.xlsx
+++ b/MSXIV_SolarSense/MSXIV_SolarSense/Project Outputs for MSXIV_SolarSense/BOM&STEP/MSXIV_SolarSense_1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aashmika Mali\Documents\First Year\Midnight Sun\hardware\MSXIV_SolarSense\MSXIV_SolarSense\Project Outputs for MSXIV_SolarSense\BOM&amp;STEP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71633F34-01DD-4979-8299-0A4F0E46AA56}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{01A3B74E-250C-4E28-A5F8-E7CC200D4FC3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3804" yWindow="2688" windowWidth="16440" windowHeight="9420" xr2:uid="{B55FF0AA-97F8-4202-BEE9-04AD2087785E}"/>
+    <workbookView xWindow="3804" yWindow="2688" windowWidth="16440" windowHeight="9420" xr2:uid="{029B0227-5933-4925-BFCD-0D8A7ED4E280}"/>
   </bookViews>
   <sheets>
     <sheet name="MSXIV_SolarSense_1.0" sheetId="1" r:id="rId1"/>
@@ -1201,7 +1201,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F50CE05-9DBB-422C-BA07-6936B5A5A92F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F42B3A2C-3BAE-4C1A-9EB0-60A3B52D8EA4}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>

<commit_message>
fixed orientation of connectors and regenerated all ouput files
</commit_message>
<xml_diff>
--- a/MSXIV_SolarSense/MSXIV_SolarSense/Project Outputs for MSXIV_SolarSense/BOM&STEP/MSXIV_SolarSense_1.0.xlsx
+++ b/MSXIV_SolarSense/MSXIV_SolarSense/Project Outputs for MSXIV_SolarSense/BOM&STEP/MSXIV_SolarSense_1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aashmika Mali\Documents\First Year\Midnight Sun\hardware\MSXIV_SolarSense\MSXIV_SolarSense\Project Outputs for MSXIV_SolarSense\BOM&amp;STEP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01A3B74E-250C-4E28-A5F8-E7CC200D4FC3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{125188D3-3E60-4DF6-BF11-EB0165849AC7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3804" yWindow="2688" windowWidth="16440" windowHeight="9420" xr2:uid="{029B0227-5933-4925-BFCD-0D8A7ED4E280}"/>
+    <workbookView xWindow="3804" yWindow="2688" windowWidth="16440" windowHeight="9420" xr2:uid="{51127C21-A574-4C78-B6DD-5D5BE454ECDC}"/>
   </bookViews>
   <sheets>
     <sheet name="MSXIV_SolarSense_1.0" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="263">
   <si>
     <t>Comment</t>
   </si>
@@ -430,6 +430,9 @@
   </si>
   <si>
     <t>CONN, 5POS MICRO-FIT 3mm</t>
+  </si>
+  <si>
+    <t>WM1925-ND</t>
   </si>
   <si>
     <t>CONN 8POS MICRO-FIT 3mm</t>
@@ -1201,7 +1204,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F42B3A2C-3BAE-4C1A-9EB0-60A3B52D8EA4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F558B4-75A6-41B0-BB3C-C995015DD9D3}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2003,29 +2006,33 @@
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="I23" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
+      <c r="L23" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
     </row>
     <row r="24" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
@@ -2038,7 +2045,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
@@ -2046,19 +2053,19 @@
     </row>
     <row r="25" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="F25" s="4">
         <v>1</v>
@@ -2071,7 +2078,7 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
@@ -2079,19 +2086,19 @@
     </row>
     <row r="26" spans="1:15" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
@@ -2104,7 +2111,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
@@ -2112,19 +2119,19 @@
     </row>
     <row r="27" spans="1:15" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="F27" s="4">
         <v>2</v>
@@ -2137,7 +2144,7 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -2145,28 +2152,28 @@
     </row>
     <row r="28" spans="1:15" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="F28" s="4">
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>19</v>
@@ -2174,7 +2181,7 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -2182,28 +2189,28 @@
     </row>
     <row r="29" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="F29" s="4">
         <v>6</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>19</v>
@@ -2211,7 +2218,7 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -2219,28 +2226,28 @@
     </row>
     <row r="30" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="F30" s="4">
         <v>7</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>19</v>
@@ -2248,7 +2255,7 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -2256,28 +2263,28 @@
     </row>
     <row r="31" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="F31" s="4">
         <v>6</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>19</v>
@@ -2285,7 +2292,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
@@ -2293,28 +2300,28 @@
     </row>
     <row r="32" spans="1:15" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="F32" s="4">
         <v>3</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>19</v>
@@ -2322,7 +2329,7 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
@@ -2330,19 +2337,19 @@
     </row>
     <row r="33" spans="1:15" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F33" s="4">
         <v>15</v>
@@ -2355,7 +2362,7 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -2363,28 +2370,28 @@
     </row>
     <row r="34" spans="1:15" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="F34" s="4">
         <v>6</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>19</v>
@@ -2392,7 +2399,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -2400,19 +2407,19 @@
     </row>
     <row r="35" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F35" s="4">
         <v>2</v>
@@ -2425,7 +2432,7 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
@@ -2433,28 +2440,28 @@
     </row>
     <row r="36" spans="1:15" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>196</v>
-      </c>
       <c r="F36" s="4">
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>19</v>
@@ -2462,7 +2469,7 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
@@ -2470,19 +2477,19 @@
     </row>
     <row r="37" spans="1:15" ht="216" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="F37" s="4">
         <v>1</v>
@@ -2495,7 +2502,7 @@
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
@@ -2503,19 +2510,19 @@
     </row>
     <row r="38" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>193</v>
-      </c>
       <c r="E38" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F38" s="4">
         <v>1</v>
@@ -2528,7 +2535,7 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
@@ -2536,19 +2543,19 @@
     </row>
     <row r="39" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>206</v>
       </c>
       <c r="F39" s="4">
         <v>1</v>
@@ -2565,19 +2572,19 @@
     </row>
     <row r="40" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F40" s="4">
         <v>1</v>
@@ -2594,19 +2601,19 @@
     </row>
     <row r="41" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F41" s="4">
         <v>1</v>
@@ -2623,19 +2630,19 @@
     </row>
     <row r="42" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F42" s="4">
         <v>1</v>
@@ -2652,19 +2659,19 @@
     </row>
     <row r="43" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F43" s="4">
         <v>6</v>
@@ -2681,19 +2688,19 @@
     </row>
     <row r="44" spans="1:15" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="F44" s="4">
         <v>1</v>
@@ -2706,7 +2713,7 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
@@ -2714,19 +2721,19 @@
     </row>
     <row r="45" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>224</v>
       </c>
       <c r="F45" s="4">
         <v>1</v>
@@ -2739,7 +2746,7 @@
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
       <c r="L45" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
@@ -2747,19 +2754,19 @@
     </row>
     <row r="46" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>229</v>
       </c>
       <c r="F46" s="4">
         <v>7</v>
@@ -2772,7 +2779,7 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
@@ -2781,16 +2788,16 @@
     <row r="47" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F47" s="4">
         <v>1</v>
@@ -2803,7 +2810,7 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
@@ -2811,28 +2818,28 @@
     </row>
     <row r="48" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="F48" s="4">
         <v>6</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="I48" s="3" t="s">
         <v>19</v>
@@ -2840,7 +2847,7 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
@@ -2848,36 +2855,36 @@
     </row>
     <row r="49" spans="1:15" ht="216" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>246</v>
       </c>
       <c r="F49" s="4">
         <v>6</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
@@ -2885,19 +2892,19 @@
     </row>
     <row r="50" spans="1:15" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="F50" s="4">
         <v>6</v>
@@ -2910,7 +2917,7 @@
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
@@ -2918,19 +2925,19 @@
     </row>
     <row r="51" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>257</v>
       </c>
       <c r="F51" s="4">
         <v>1</v>
@@ -2943,7 +2950,7 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>

</xml_diff>

<commit_message>
fixed silkscreen on pcb a bit
</commit_message>
<xml_diff>
--- a/MSXIV_SolarSense/MSXIV_SolarSense/Project Outputs for MSXIV_SolarSense/BOM&STEP/MSXIV_SolarSense_1.0.xlsx
+++ b/MSXIV_SolarSense/MSXIV_SolarSense/Project Outputs for MSXIV_SolarSense/BOM&STEP/MSXIV_SolarSense_1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aashmika Mali\Documents\First Year\Midnight Sun\hardware\MSXIV_SolarSense\MSXIV_SolarSense\Project Outputs for MSXIV_SolarSense\BOM&amp;STEP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75C8BBE4-19E9-46C4-B2E3-9B40D333EEB7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73570AD5-DCF2-4CDB-9EED-4A6E888A3C2F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3804" yWindow="2688" windowWidth="16440" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1008" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Report" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="216">
   <si>
     <t>Title</t>
   </si>
@@ -511,9 +511,6 @@
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>RSComponents</t>
-  </si>
-  <si>
     <t>TI store</t>
   </si>
   <si>
@@ -674,6 +671,12 @@
   </si>
   <si>
     <t>BOM</t>
+  </si>
+  <si>
+    <t>DDZ9699DICT-ND</t>
+  </si>
+  <si>
+    <t>Digi-key</t>
   </si>
 </sst>
 </file>
@@ -858,20 +861,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1248,8 +1251,8 @@
   </sheetPr>
   <dimension ref="A2:J64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1267,10 +1270,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="27"/>
       <c r="D2" s="2"/>
     </row>
@@ -1278,7 +1281,7 @@
       <c r="A3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1286,7 +1289,7 @@
       <c r="A4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1294,7 +1297,7 @@
       <c r="A5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="5"/>
@@ -1307,7 +1310,7 @@
       <c r="A6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="5"/>
@@ -1320,7 +1323,7 @@
       <c r="A7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="24"/>
@@ -1330,7 +1333,7 @@
       <c r="A8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="24"/>
@@ -1339,7 +1342,7 @@
       <c r="A9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="24"/>
@@ -1364,16 +1367,16 @@
         <v>158</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G11" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="H11" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="I11" s="21" t="s">
         <v>206</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1389,7 +1392,7 @@
         <v>159</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3">
@@ -1414,7 +1417,7 @@
         <v>159</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3">
@@ -1439,7 +1442,7 @@
         <v>159</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3">
@@ -1460,7 +1463,7 @@
         <v>159</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3">
@@ -1485,7 +1488,7 @@
         <v>159</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3">
@@ -1506,7 +1509,7 @@
         <v>159</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3">
@@ -1531,7 +1534,7 @@
         <v>159</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3">
@@ -1556,7 +1559,7 @@
         <v>159</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3">
@@ -1581,7 +1584,7 @@
         <v>159</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3">
@@ -1606,7 +1609,7 @@
         <v>159</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3">
@@ -1627,7 +1630,7 @@
         <v>159</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3">
@@ -1645,10 +1648,10 @@
       <c r="C23" s="4"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="F23" s="9">
-        <v>8222413</v>
+        <v>215</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>214</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3">
@@ -1669,7 +1672,7 @@
         <v>159</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3">
@@ -1690,7 +1693,7 @@
         <v>159</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3">
@@ -1711,7 +1714,7 @@
         <v>159</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3">
@@ -1732,7 +1735,7 @@
         <v>159</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3">
@@ -1753,7 +1756,7 @@
         <v>159</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3">
@@ -1774,7 +1777,7 @@
         <v>159</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3">
@@ -1799,7 +1802,7 @@
         <v>159</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3">
@@ -1820,7 +1823,7 @@
         <v>159</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3">
@@ -1841,7 +1844,7 @@
         <v>159</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3">
@@ -1862,7 +1865,7 @@
         <v>159</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3">
@@ -1883,7 +1886,7 @@
         <v>159</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3">
@@ -1904,7 +1907,7 @@
         <v>159</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3">
@@ -1925,7 +1928,7 @@
         <v>159</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3">
@@ -1946,7 +1949,7 @@
         <v>159</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3">
@@ -1971,7 +1974,7 @@
         <v>159</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3">
@@ -1996,7 +1999,7 @@
         <v>159</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3">
@@ -2021,7 +2024,7 @@
         <v>159</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3">
@@ -2046,7 +2049,7 @@
         <v>159</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3">
@@ -2071,7 +2074,7 @@
         <v>159</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3">
@@ -2092,7 +2095,7 @@
         <v>159</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3">
@@ -2117,7 +2120,7 @@
         <v>159</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3">
@@ -2138,7 +2141,7 @@
         <v>159</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3">
@@ -2163,7 +2166,7 @@
         <v>159</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3">
@@ -2184,7 +2187,7 @@
         <v>159</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3">
@@ -2205,7 +2208,7 @@
         <v>159</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3">
@@ -2311,7 +2314,7 @@
         <v>159</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3">
@@ -2332,7 +2335,7 @@
         <v>159</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3">
@@ -2353,7 +2356,7 @@
         <v>159</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3">
@@ -2374,7 +2377,7 @@
         <v>159</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3">
@@ -2399,7 +2402,7 @@
         <v>159</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3">
@@ -2421,7 +2424,7 @@
         <v>157</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>157</v>
@@ -2445,7 +2448,7 @@
         <v>159</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3">
@@ -2466,7 +2469,7 @@
         <v>159</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3">
@@ -2551,15 +2554,15 @@
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32" t="s">
-        <v>208</v>
+      <c r="B1" s="31" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2567,15 +2570,15 @@
       <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>209</v>
+      <c r="B3" s="31" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2583,23 +2586,23 @@
       <c r="A5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>208</v>
+      <c r="B5" s="31" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>210</v>
+      <c r="B6" s="31" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2607,23 +2610,23 @@
       <c r="A8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>211</v>
+      <c r="B8" s="31" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>212</v>
+      <c r="B9" s="31" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2631,7 +2634,7 @@
       <c r="A11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2639,23 +2642,23 @@
       <c r="A12" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>213</v>
+      <c r="B12" s="31" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>214</v>
+      <c r="B13" s="31" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="31" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>